<commit_message>
Update Data_description_Input_EU_2030 (compatible with current BB4).xlsx
</commit_message>
<xml_diff>
--- a/Data_description_Input_EU_2030 (compatible with current BB4).xlsx
+++ b/Data_description_Input_EU_2030 (compatible with current BB4).xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schoeniger\Documents\Github\EEG-Tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hasengst\Documents\GitHub\EEG-Tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBBBB4EF-D6FA-4F28-81B9-DFE316D30D20}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D88E4FB-F65A-46FF-91FC-804112EBA569}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10425" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="79">
   <si>
     <t>Reservoir capacity (MWh storage capacity/MW installed capacity)</t>
   </si>
@@ -78,9 +78,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Input_Austria_2030 (compatible with current BB4)</t>
-  </si>
-  <si>
     <t>Project</t>
   </si>
   <si>
@@ -105,14 +102,6 @@
     <t>Installed power plant capacities</t>
   </si>
   <si>
-    <t>Github Clean File (based on AURES II offshore case study)</t>
-  </si>
-  <si>
-    <t>Conventional: Processing tool Jasper
-Renewables: GreenX run for Offshore Hub case study AURES II
-Heat pumps: diploma thesis of Danijel Katsman</t>
-  </si>
-  <si>
     <t>Technologies characteristics</t>
   </si>
   <si>
@@ -185,9 +174,6 @@
     <t>Annual electricity consumption (MWh)</t>
   </si>
   <si>
-    <t>GreenX - autoproduction - self consumption - transport loss</t>
-  </si>
-  <si>
     <t>PARAMETER DH(YYY,AAA,DHUSER)</t>
   </si>
   <si>
@@ -195,9 +181,6 @@
   </si>
   <si>
     <t>CHP heat demand (PRIMES)</t>
-  </si>
-  <si>
-    <t>Heat demand based on PRIMES euco30 with own adaptations to meet 2030 targets (on RES and EE)</t>
   </si>
   <si>
     <t>TABLE XKFX(YYY,IRRRE,IRRRI)</t>
@@ -321,6 +304,29 @@
   </si>
   <si>
     <t>2020+2040: TYNDP2018 Distributed Generation Scenario; 2030: TYNDP2020 National Trends Scenario</t>
+  </si>
+  <si>
+    <t>2030: AURES II NECP- NoTrade Scenario; 2019: ENTSOE</t>
+  </si>
+  <si>
+    <t>GreenX - autoproduction - self consumption - transport loss; 2019 ENTSOE</t>
+  </si>
+  <si>
+    <t>2030: AURES II NECP- NoTrade Scenario; 2019: PRIMES REF2020-draft minus autoproducers</t>
+  </si>
+  <si>
+    <t>2019: scaled to ENTSOE capacities</t>
+  </si>
+  <si>
+    <t>Github Clean File (based on AURES II NECP-NoTrade scenario)</t>
+  </si>
+  <si>
+    <t>Input_EU_2030 (compatible with current BB4)</t>
+  </si>
+  <si>
+    <t>Conventional: Processing tool Jasper;
+Renewables: GreenX run for  AURES II NECP-NoTrade Scenario; 2019 data ENTSOE 
+Heat pumps: diploma thesis of Danijel Katsman                                                               Heat only Boilders: PRIMES; estimated FLH=3000</t>
   </si>
 </sst>
 </file>
@@ -1075,7 +1081,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1085,31 +1091,31 @@
         <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -1122,7 +1128,7 @@
   <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1137,53 +1143,55 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="1"/>
+        <v>78</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="3" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F3" s="1"/>
     </row>
@@ -1192,10 +1200,10 @@
         <v>21</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D4" s="5">
         <v>0.05</v>
@@ -1207,10 +1215,10 @@
         <v>21</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D5" s="4">
         <v>8.0199999999999994E-2</v>
@@ -1222,10 +1230,10 @@
         <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D6" s="4">
         <v>1</v>
@@ -1237,10 +1245,10 @@
         <v>24</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D7" s="4">
         <v>3.2000000000000001E-2</v>
@@ -1252,10 +1260,10 @@
         <v>25</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D8" s="4">
         <v>0.1</v>
@@ -1267,42 +1275,42 @@
         <v>28</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C9" s="3"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D11" s="6"/>
       <c r="F11" s="1"/>
@@ -1312,33 +1320,35 @@
         <v>33</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>34</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>43</v>
+        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1349,11 +1359,11 @@
         <v>2</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="1" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="F14" s="1"/>
     </row>
@@ -1362,10 +1372,10 @@
         <v>38</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="D15" s="6">
         <v>2.1999999999999999E-2</v>
@@ -1377,17 +1387,17 @@
         <v>39</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1395,49 +1405,49 @@
         <v>40</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="6"/>
       <c r="E18" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="6"/>
       <c r="E19" s="1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="6"/>
@@ -1497,10 +1507,13 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="10"/>
@@ -1516,10 +1529,10 @@
     </row>
     <row r="2" spans="1:12" ht="24.75" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C2" s="13">
         <f>'[1]QUO-pDEF(PVdecBAU)'!$E$12</f>
@@ -1559,10 +1572,10 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C3" s="13">
         <f>'[1]QUO-pDEF(PVdecBAU)'!$E$13</f>
@@ -1602,10 +1615,10 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B4" s="12" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C4" s="13">
         <f>'[1]QUO-pDEF(PVdecBAU)'!$E$14</f>
@@ -1645,10 +1658,10 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C5" s="13">
         <v>4</v>
@@ -1681,10 +1694,10 @@
     </row>
     <row r="6" spans="1:12" ht="62.25" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="C6" s="13">
         <f>'[1]QUO-pDEF(PVdecBAU)'!$E$15</f>
@@ -1724,19 +1737,19 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1809,16 +1822,16 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="E17" s="1"/>
     </row>

</xml_diff>